<commit_message>
Adding some omages to test in the printer
</commit_message>
<xml_diff>
--- a/spring-boot/test.xlsx
+++ b/spring-boot/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r0g01a5/Documents/mywork/bulk-barcode-generator/spring-boot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C84B7711-9039-484C-9CAB-AD879FAEE424}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36742BAB-41FC-FD4E-87E8-25A95A62A3BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -163,39 +163,35 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="fill" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares [0]" xfId="2" builtinId="6"/>
@@ -478,31 +474,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:K4"/>
+  <dimension ref="A1:J4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="10.83203125" style="8"/>
-    <col min="2" max="2" width="31" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="9" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="21.5" style="9" customWidth="1"/>
+    <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="10" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.1640625" style="8" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" style="8" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="8"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>2</v>
       </c>
       <c r="C1" s="3" t="s">
@@ -514,116 +511,114 @@
       <c r="E1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="6" t="s">
+      <c r="F1" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="15" t="s">
+      <c r="G1" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="14" t="s">
+      <c r="H1" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="11"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="8">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="9">
         <v>1140187</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="5">
+      <c r="D2" s="10">
         <v>499990</v>
       </c>
-      <c r="E2" s="5">
+      <c r="E2" s="10">
         <v>289270</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="11">
         <v>144635</v>
       </c>
-      <c r="G2" s="12">
+      <c r="G2" s="10">
         <f>F2*1.19</f>
         <v>172115.65</v>
       </c>
-      <c r="H2" s="9">
+      <c r="H2" s="10">
         <v>310000</v>
       </c>
-      <c r="I2">
+      <c r="I2" s="8">
         <v>1</v>
       </c>
-      <c r="J2" t="s">
+      <c r="J2" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A3" s="8">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="9">
         <v>1105689</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="8" t="s">
         <v>5</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="5">
+      <c r="D3" s="10">
         <v>549990</v>
       </c>
-      <c r="E3" s="5">
+      <c r="E3" s="10">
         <v>358312</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="11">
         <v>179156</v>
       </c>
-      <c r="G3" s="12">
+      <c r="G3" s="10">
         <f t="shared" ref="G3:G4" si="0">F3*1.19</f>
         <v>213195.63999999998</v>
       </c>
-      <c r="H3" s="9">
+      <c r="H3" s="10">
         <v>320000</v>
       </c>
-      <c r="I3">
+      <c r="I3" s="8">
         <v>1</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3" s="8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A4" s="8">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="9">
         <v>1100625</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="5">
+      <c r="D4" s="10">
         <v>259990</v>
       </c>
-      <c r="E4" s="5">
+      <c r="E4" s="10">
         <v>163354</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="11">
         <v>81677</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="10">
         <f t="shared" si="0"/>
         <v>97195.62999999999</v>
       </c>
-      <c r="H4" s="9">
+      <c r="H4" s="10">
         <v>150000</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="8">
         <v>1</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="K4" s="13"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:J4" xr:uid="{00000000-0009-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Adding zip file generator
</commit_message>
<xml_diff>
--- a/spring-boot/test.xlsx
+++ b/spring-boot/test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/r0g01a5/Documents/mywork/bulk-barcode-generator/spring-boot/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0E6F39E1-7F5A-2440-9676-B9FFB36D0AC7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53E55569-67C2-8743-B486-FC8EB0975C47}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="34560" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="23">
   <si>
     <t>Lavadora Secadora Perfect Care</t>
   </si>
@@ -83,15 +83,6 @@
     <t>112345678</t>
   </si>
   <si>
-    <t>50000</t>
-  </si>
-  <si>
-    <t>399990</t>
-  </si>
-  <si>
-    <t>1200</t>
-  </si>
-  <si>
     <t>BOWSER</t>
   </si>
   <si>
@@ -117,12 +108,6 @@
   </si>
   <si>
     <t>REGLA</t>
-  </si>
-  <si>
-    <t>30000</t>
-  </si>
-  <si>
-    <t>42000</t>
   </si>
 </sst>
 </file>
@@ -208,8 +193,12 @@
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
@@ -226,9 +215,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="4" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -522,282 +508,282 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="21.5" style="9" customWidth="1"/>
-    <col min="2" max="2" width="31" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="15.1640625" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17.83203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.33203125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.1640625" style="8" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.33203125" style="8" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="10.83203125" style="8"/>
+    <col min="1" max="1" width="21.5" style="10" customWidth="1"/>
+    <col min="2" max="2" width="31" style="9" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="15.1640625" style="11" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.83203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.33203125" style="12" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.1640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.33203125" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="10.83203125" style="9"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="D1" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="E1" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="5" t="s">
+      <c r="F1" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="6" t="s">
+      <c r="G1" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="7" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="9">
+      <c r="A2" s="10">
         <v>1140187</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10">
+      <c r="D2" s="11">
         <v>499990</v>
       </c>
-      <c r="E2" s="10">
+      <c r="E2" s="11">
         <v>289270</v>
       </c>
-      <c r="F2" s="11">
+      <c r="F2" s="12">
         <v>144635</v>
       </c>
-      <c r="G2" s="10">
+      <c r="G2" s="11">
         <f>F2*1.19</f>
         <v>172115.65</v>
       </c>
-      <c r="H2" s="10">
+      <c r="H2" s="1">
         <v>310000</v>
       </c>
-      <c r="I2" s="8">
+      <c r="I2" s="9">
         <v>1</v>
       </c>
-      <c r="J2" s="8" t="s">
+      <c r="J2" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="9">
+      <c r="A3" s="10">
         <v>1105689</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10">
+      <c r="D3" s="11">
         <v>549990</v>
       </c>
-      <c r="E3" s="10">
+      <c r="E3" s="11">
         <v>358312</v>
       </c>
-      <c r="F3" s="11">
+      <c r="F3" s="12">
         <v>179156</v>
       </c>
-      <c r="G3" s="10">
+      <c r="G3" s="11">
         <f t="shared" ref="G3:G9" si="0">F3*1.19</f>
         <v>213195.63999999998</v>
       </c>
-      <c r="H3" s="10">
+      <c r="H3" s="1">
         <v>320000</v>
       </c>
-      <c r="I3" s="8">
+      <c r="I3" s="9">
         <v>1</v>
       </c>
-      <c r="J3" s="8" t="s">
+      <c r="J3" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="9">
+      <c r="A4" s="10">
         <v>1100625</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="10">
+      <c r="D4" s="11">
         <v>259990</v>
       </c>
-      <c r="E4" s="10">
+      <c r="E4" s="11">
         <v>163354</v>
       </c>
-      <c r="F4" s="11">
+      <c r="F4" s="12">
         <v>81677</v>
       </c>
-      <c r="G4" s="10">
+      <c r="G4" s="11">
         <f t="shared" si="0"/>
         <v>97195.62999999999</v>
       </c>
-      <c r="H4" s="10">
+      <c r="H4" s="1">
         <v>150000</v>
       </c>
-      <c r="I4" s="8">
+      <c r="I4" s="9">
         <v>1</v>
       </c>
-      <c r="J4" s="8" t="s">
+      <c r="J4" s="9" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="B5" s="8" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="8" t="s">
+      <c r="B5" s="9" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D5" s="10">
+      <c r="D5" s="11">
         <v>499990</v>
       </c>
-      <c r="E5" s="10">
+      <c r="E5" s="11">
         <v>289270</v>
       </c>
-      <c r="F5" s="11">
+      <c r="F5" s="12">
         <v>144635</v>
       </c>
-      <c r="G5" s="10">
+      <c r="G5" s="11">
         <f>F5*1.19</f>
         <v>172115.65</v>
       </c>
-      <c r="H5" s="10" t="s">
+      <c r="H5" s="1">
+        <v>50000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="B6" s="9" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B6" s="8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D6" s="10">
+      <c r="D6" s="11">
         <v>549990</v>
       </c>
-      <c r="E6" s="10">
+      <c r="E6" s="11">
         <v>358312</v>
       </c>
-      <c r="F6" s="11">
+      <c r="F6" s="12">
         <v>179156</v>
       </c>
-      <c r="G6" s="10">
+      <c r="G6" s="11">
         <f t="shared" si="0"/>
         <v>213195.63999999998</v>
       </c>
-      <c r="H6" s="10" t="s">
-        <v>15</v>
+      <c r="H6" s="1">
+        <v>399990</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="8" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="8" t="s">
+      <c r="A7" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D7" s="10">
+      <c r="D7" s="11">
         <v>259990</v>
       </c>
-      <c r="E7" s="10">
+      <c r="E7" s="11">
         <v>163354</v>
       </c>
-      <c r="F7" s="11">
+      <c r="F7" s="12">
         <v>81677</v>
       </c>
-      <c r="G7" s="10">
+      <c r="G7" s="11">
         <f t="shared" si="0"/>
         <v>97195.62999999999</v>
       </c>
-      <c r="H7" s="10" t="s">
-        <v>16</v>
+      <c r="H7" s="1">
+        <v>1200</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B8" s="8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" s="8" t="s">
+      <c r="A8" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B8" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="11">
         <v>499990</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="11">
         <v>289270</v>
       </c>
-      <c r="F8" s="11">
+      <c r="F8" s="12">
         <v>144635</v>
       </c>
-      <c r="G8" s="10">
+      <c r="G8" s="11">
         <f>F8*1.19</f>
         <v>172115.65</v>
       </c>
-      <c r="H8" s="10" t="s">
-        <v>27</v>
+      <c r="H8" s="1">
+        <v>42000</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="9" t="s">
-        <v>24</v>
-      </c>
-      <c r="B9" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="C9" s="8" t="s">
+      <c r="A9" s="10" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="9" t="s">
+        <v>22</v>
+      </c>
+      <c r="C9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="D9" s="10">
+      <c r="D9" s="11">
         <v>549990</v>
       </c>
-      <c r="E9" s="10">
+      <c r="E9" s="11">
         <v>358312</v>
       </c>
-      <c r="F9" s="11">
+      <c r="F9" s="12">
         <v>179156</v>
       </c>
-      <c r="G9" s="10">
+      <c r="G9" s="11">
         <f t="shared" si="0"/>
         <v>213195.63999999998</v>
       </c>
-      <c r="H9" s="10" t="s">
-        <v>26</v>
+      <c r="H9" s="1">
+        <v>30000</v>
       </c>
     </row>
   </sheetData>

</xml_diff>